<commit_message>
analysis of category "uncertain" for system understanding added
</commit_message>
<xml_diff>
--- a/data/results/00_readme_tables+figures.xlsx
+++ b/data/results/00_readme_tables+figures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga84kuj\Documents\R\VDA_FOT\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4CF5E3-2486-4738-B690-E11036A4F38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0AFF09-B584-4E7B-9FE2-F313781B0F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D11BFDDA-6A65-4D99-AF95-D04BA2DC2326}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
   <si>
     <t>Kategorie</t>
   </si>
@@ -204,15 +204,7 @@
     <t>- s. summary_nachbefragung</t>
   </si>
   <si>
-    <t>CTAM</t>
-  </si>
-  <si>
     <t>System_sum</t>
-  </si>
-  <si>
-    <t>- Score aus den 16 Fragen. Berechnet wurde, wie viele korrekt waren.
-- als Graphik ist auch nochmal aufgeschlüsselt, welche Fragen zu viel Prozent korrekt beantwortet wurden
-- bisher unberücksichtigt ist die Angabe "unsicher". Sie wird bisher als falsch gewertet. Hier sollten wir noch die Auswertung ergänzen</t>
   </si>
   <si>
     <t>NDRT…</t>
@@ -329,6 +321,26 @@
   <si>
     <t>CTAM
 --&gt; see literature_scales</t>
+  </si>
+  <si>
+    <t>System_u_*</t>
+  </si>
+  <si>
+    <t>- Score aus den 16 Fragen. Berechnet wurde, wie viele korrekt waren.
+- als Graphik ist auch nochmal aufgeschlüsselt, welche Fragen zu viel Prozent korrekt beantwortet wurden
+- die Angabe "unsicher" wird hier als falsch gewertet. Die Anzahl der Nennungen "unsicher" findet sich in der Tabelle frequencies_nachbefragung System_u_...</t>
+  </si>
+  <si>
+    <t>falsch</t>
+  </si>
+  <si>
+    <t>richtig</t>
+  </si>
+  <si>
+    <t>die Angabe "unsicher" wird beim System_sum als falsch gewertet. Die Anzahl der Nennungen "unsicher" findet sich hier aufgeschlüsselt nach den einzelnen Fragen 1-16
+7x in Intervall A_on_fc (aber alles von nur zwei VP03 (4x, items 1, 3, 15, 16) und 12(3x, items 1, 11, 16),
+2x in Intervall A_on_fam (beides VP12: items 1, 16)
+0x in A_off und B_off</t>
   </si>
 </sst>
 </file>
@@ -390,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -433,6 +445,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -749,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464E2BF1-EB53-4C42-B8DA-8D95C1EDEE80}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +812,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -847,10 +862,10 @@
     </row>
     <row r="6" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -862,10 +877,10 @@
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1136,10 +1151,10 @@
     </row>
     <row r="21" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -1151,10 +1166,10 @@
     </row>
     <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -1166,10 +1181,10 @@
     </row>
     <row r="23" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -1181,36 +1196,36 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="H24" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="I24" s="11"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
@@ -1218,16 +1233,16 @@
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>24</v>
@@ -1240,60 +1255,60 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="G27" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="G28" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
@@ -1301,6 +1316,27 @@
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
     </row>
+    <row r="30" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update SU + graphics
</commit_message>
<xml_diff>
--- a/data/results/00_readme_tables+figures.xlsx
+++ b/data/results/00_readme_tables+figures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ga84kuj\Documents\R\VDA_FOT\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0AFF09-B584-4E7B-9FE2-F313781B0F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74B2662-1B7F-4B8E-98B8-609E7A808540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D11BFDDA-6A65-4D99-AF95-D04BA2DC2326}"/>
   </bookViews>
@@ -337,10 +337,7 @@
     <t>richtig</t>
   </si>
   <si>
-    <t>die Angabe "unsicher" wird beim System_sum als falsch gewertet. Die Anzahl der Nennungen "unsicher" findet sich hier aufgeschlüsselt nach den einzelnen Fragen 1-16
-7x in Intervall A_on_fc (aber alles von nur zwei VP03 (4x, items 1, 3, 15, 16) und 12(3x, items 1, 11, 16),
-2x in Intervall A_on_fam (beides VP12: items 1, 16)
-0x in A_off und B_off</t>
+    <t>die Angabe "unsicher" wird beim System_sum als falsch gewertet. Die Anzahl der Nennungen "unsicher" findet sich hier aufgeschlüsselt nach den einzelnen Fragen 1-16</t>
   </si>
 </sst>
 </file>
@@ -370,7 +367,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,6 +386,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -402,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -422,7 +431,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -435,19 +443,38 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -766,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464E2BF1-EB53-4C42-B8DA-8D95C1EDEE80}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,531 +838,386 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    </row>
+    <row r="6" spans="1:9" s="13" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    </row>
+    <row r="7" spans="1:9" s="13" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    </row>
+    <row r="8" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    </row>
+    <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    </row>
+    <row r="10" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    </row>
+    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    </row>
+    <row r="12" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    </row>
+    <row r="13" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    </row>
+    <row r="14" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    </row>
+    <row r="15" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    </row>
+    <row r="16" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    </row>
+    <row r="17" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    </row>
+    <row r="18" spans="1:9" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+    </row>
+    <row r="19" spans="1:9" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    </row>
+    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-    </row>
-    <row r="21" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+    </row>
+    <row r="21" spans="1:9" s="18" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-    </row>
-    <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+    </row>
+    <row r="22" spans="1:9" s="18" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+    </row>
+    <row r="23" spans="1:9" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+    </row>
+    <row r="24" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="I24" s="11"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+    </row>
+    <row r="25" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+    </row>
+    <row r="27" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+    </row>
+    <row r="28" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    </row>
+    <row r="29" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-    </row>
-    <row r="30" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+    </row>
+    <row r="30" spans="1:9" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="D30" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>